<commit_message>
updated some tables, made a prettier FIFO trend figure
</commit_message>
<xml_diff>
--- a/tables/TableS11_feed_scenarios.xlsx
+++ b/tables/TableS11_feed_scenarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/aquacast/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A37FFBF-A141-0C41-8DDA-30AEF658283C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B106982D-1CAB-E746-9915-12B2C19B6113}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20860" yWindow="10700" windowWidth="25600" windowHeight="15540" xr2:uid="{111A2066-40EB-7F4F-8231-647CE8CF5F93}"/>
+    <workbookView xWindow="17440" yWindow="2360" windowWidth="25600" windowHeight="15540" xr2:uid="{111A2066-40EB-7F4F-8231-647CE8CF5F93}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,17 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>BAU fisheries management</t>
   </si>
   <si>
-    <t>Current FM/FO compositions</t>
-  </si>
-  <si>
-    <t>Current feed conversion rates</t>
-  </si>
-  <si>
     <t>Not evaluated due to lack of data</t>
   </si>
   <si>
@@ -54,9 +48,6 @@
     <t>4. Reduce the feed conversion rate (i.e., increase feed efficiency)</t>
   </si>
   <si>
-    <t>Base case scenario</t>
-  </si>
-  <si>
     <t>Progressive reform scenario</t>
   </si>
   <si>
@@ -69,25 +60,46 @@
     <t>a. Reduce use in non-carnivorous terrestrial agriculture</t>
   </si>
   <si>
-    <t xml:space="preserve">75% of forage fish to aquaculture </t>
-  </si>
-  <si>
-    <t>75% of forage fish to aquaculture</t>
-  </si>
-  <si>
     <t>b. Reduce use in non-carnivorous fish aquaculture</t>
   </si>
   <si>
-    <t>28% of aquaculture feed to mariculture</t>
-  </si>
-  <si>
-    <t>100% of aquaculture feed to mariculture</t>
-  </si>
-  <si>
-    <t>FIFO ratios projected for 2050</t>
-  </si>
-  <si>
     <t>Pathway</t>
+  </si>
+  <si>
+    <t>2030 FM/FO compositions</t>
+  </si>
+  <si>
+    <t>2030 feed conversion rates</t>
+  </si>
+  <si>
+    <t>2050 FM/FO compositions</t>
+  </si>
+  <si>
+    <t>2050 feed conversion rates</t>
+  </si>
+  <si>
+    <t>Business-as-usual scenario</t>
+  </si>
+  <si>
+    <t>100% of this supply to mariculture</t>
+  </si>
+  <si>
+    <t>Percent of forage fish destined for reduction to mariculture:</t>
+  </si>
+  <si>
+    <t>21.2% of forage fish to mariculture</t>
+  </si>
+  <si>
+    <t>74.5% of forage fish to mariculture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">74.5% of forage fish to aquaculture </t>
+  </si>
+  <si>
+    <t>74.5% of forage fish to aquaculture</t>
+  </si>
+  <si>
+    <t>28.5% of this supply to mariculture</t>
   </si>
 </sst>
 </file>
@@ -157,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -170,6 +182,9 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -486,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70231C1-8536-E847-89C1-FD432232D7EB}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -502,93 +517,119 @@
     <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="A7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>